<commit_message>
prepped READMEdriven development lecture
</commit_message>
<xml_diff>
--- a/CIS440FALL2014schedule.xlsx
+++ b/CIS440FALL2014schedule.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="145">
   <si>
     <t>topic</t>
   </si>
@@ -132,18 +132,12 @@
     <t>tech talk #2a,2b</t>
   </si>
   <si>
-    <t>tech talk #3a,3b</t>
-  </si>
-  <si>
     <t>tech talk #4a,4b</t>
   </si>
   <si>
     <t>tech talk #5a,5b</t>
   </si>
   <si>
-    <t>tech talk #6a,6b</t>
-  </si>
-  <si>
     <t>intro</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>testing, devops</t>
   </si>
   <si>
-    <t>collaboration, project management</t>
-  </si>
-  <si>
     <t>agility &amp; discipline</t>
   </si>
   <si>
@@ -285,15 +276,9 @@
     <t>pp. 51-64</t>
   </si>
   <si>
-    <t>pp. 65-98</t>
-  </si>
-  <si>
     <t>pp. 137-177</t>
   </si>
   <si>
-    <t>tinyurl.com/8nzabtz</t>
-  </si>
-  <si>
     <t>youtu.be/ILkT_HV9DVU</t>
   </si>
   <si>
@@ -333,9 +318,6 @@
     <t>new lecture -- maybe use Travis CI?</t>
   </si>
   <si>
-    <t>digital marketing, consulting, etc</t>
-  </si>
-  <si>
     <t>send second questionnaire</t>
   </si>
   <si>
@@ -375,9 +357,6 @@
     <t>some video</t>
   </si>
   <si>
-    <t>pp. 99-136 + youtu.be/V5p8m1IjJoA</t>
-  </si>
-  <si>
     <t>Joshua Kerievsky on Lean Startup vs. Agile development</t>
   </si>
   <si>
@@ -399,9 +378,6 @@
     <t>Sims + Johnson scrum video</t>
   </si>
   <si>
-    <t>VIDEO demo day (prof. out of town)</t>
-  </si>
-  <si>
     <t>pp. 9-20 + youtu.be/NP9AIUT9nos</t>
   </si>
   <si>
@@ -439,9 +415,6 @@
   </si>
   <si>
     <t>teal = not finalized, check later</t>
-  </si>
-  <si>
-    <t>possible 29th drive guest workshop on UX design today or thurs</t>
   </si>
   <si>
     <t>guest lecture: Ray Stacey of Sogeti</t>
@@ -472,12 +445,56 @@
       <t>have course assignments defined by this date</t>
     </r>
   </si>
+  <si>
+    <t>pp. 65-98 + tinyurl.com/8nzabtz</t>
+  </si>
+  <si>
+    <t>youtu.be/V5p8m1IjJoA</t>
+  </si>
+  <si>
+    <t>pp. 99-136</t>
+  </si>
+  <si>
+    <t>guest workshop: 29th Drive</t>
+  </si>
+  <si>
+    <t>guest workshop on "agile usability testing" with UX design</t>
+  </si>
+  <si>
+    <t>demo day #4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>video</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tech talks (#3a,3b) - prof. out of town</t>
+    </r>
+  </si>
+  <si>
+    <t>collaboration, proj. mgmt., digital marketing, consulting, etc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,6 +588,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -772,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -940,6 +965,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1254,7 +1282,7 @@
   <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,7 +1316,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="39" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1"/>
@@ -1304,25 +1332,25 @@
         <v>0</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="62" t="s">
-        <v>135</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1333,18 +1361,18 @@
         <v>41872</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="55" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="8" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="37" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1355,17 +1383,17 @@
         <v>41877</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="8" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="58" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1374,18 +1402,18 @@
         <v>41879</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="9" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G6" s="58"/>
       <c r="H6" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1396,14 +1424,14 @@
         <v>41884</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="37" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="G7" s="59"/>
     </row>
@@ -1415,18 +1443,18 @@
       <c r="C8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="35" t="s">
-        <v>111</v>
+      <c r="D8" s="36" t="s">
+        <v>105</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G8" s="58"/>
       <c r="H8" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1437,20 +1465,21 @@
         <v>41891</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>87</v>
+        <v>48</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>137</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>62</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F9" s="10"/>
       <c r="G9" s="58"/>
+      <c r="H9" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="I9" s="43" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J9" s="43">
         <v>5</v>
@@ -1464,16 +1493,16 @@
       <c r="C10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>89</v>
+      <c r="D10" s="36" t="s">
+        <v>138</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G10" s="58"/>
       <c r="H10" s="8" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1483,20 +1512,17 @@
       <c r="B11" s="20">
         <v>41898</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>52</v>
+      <c r="C11" s="66" t="s">
+        <v>140</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G11" s="58"/>
-      <c r="H11" s="8" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="12" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
@@ -1506,15 +1532,15 @@
       <c r="C12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="55" t="s">
-        <v>123</v>
+      <c r="D12" s="36" t="s">
+        <v>116</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G12" s="58"/>
       <c r="H12" s="38" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1524,21 +1550,21 @@
       <c r="B13" s="20">
         <v>41905</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>35</v>
+      <c r="C13" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G13" s="58"/>
       <c r="I13" s="43" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J13" s="43">
         <v>5</v>
@@ -1550,23 +1576,23 @@
         <v>41907</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G14" s="60"/>
       <c r="H14" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="J14" s="42">
         <v>5</v>
@@ -1580,20 +1606,20 @@
         <v>41912</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="9" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="G15" s="58" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1606,7 +1632,7 @@
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G16" s="58"/>
     </row>
@@ -1618,21 +1644,21 @@
         <v>41919</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="54"/>
       <c r="E17" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G17" s="58" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H17" s="38"/>
       <c r="I17" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J17" s="43">
         <v>5</v>
@@ -1644,18 +1670,18 @@
         <v>41921</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G18" s="59"/>
       <c r="H18" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1678,20 +1704,20 @@
         <v>41928</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="D20" s="55" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G20" s="59"/>
       <c r="H20" s="37" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1702,23 +1728,23 @@
         <v>41933</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="D21" s="63" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G21" s="59"/>
       <c r="H21" s="38" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I21" s="43" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J21" s="43">
         <v>5</v>
@@ -1730,20 +1756,18 @@
         <v>41935</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="50" t="s">
-        <v>130</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E22" s="50"/>
       <c r="F22" s="9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G22" s="64"/>
       <c r="I22" s="42" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="J22" s="42">
         <v>12</v>
@@ -1757,14 +1781,14 @@
         <v>41940</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G23" s="59"/>
     </row>
@@ -1778,7 +1802,7 @@
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G24" s="59"/>
     </row>
@@ -1790,20 +1814,20 @@
         <v>41947</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D25" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G25" s="59"/>
       <c r="I25" s="43" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J25" s="43">
         <v>5</v>
@@ -1815,14 +1839,14 @@
         <v>41949</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G26" s="59"/>
     </row>
@@ -1850,7 +1874,7 @@
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G28" s="59"/>
     </row>
@@ -1862,20 +1886,20 @@
         <v>41961</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D29" s="56" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="G29" s="59"/>
       <c r="I29" s="43" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J29" s="43">
         <v>5</v>
@@ -1887,18 +1911,18 @@
         <v>41963</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G30" s="59"/>
       <c r="H30" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1909,15 +1933,15 @@
         <v>41968</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="51" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G31" s="64"/>
       <c r="I31" s="42" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="J31" s="42">
         <v>8</v>
@@ -1932,10 +1956,12 @@
         <v>25</v>
       </c>
       <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
+      <c r="E32" s="67" t="s">
+        <v>122</v>
+      </c>
       <c r="G32" s="59"/>
       <c r="I32" s="44" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J32" s="44">
         <v>8</v>
@@ -1953,11 +1979,11 @@
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="40" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G33" s="65"/>
       <c r="I33" s="43" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J33" s="43">
         <v>8</v>
@@ -1969,20 +1995,20 @@
         <v>41977</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G34" s="61"/>
       <c r="I34" s="43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J34" s="43">
         <v>10</v>
@@ -2002,7 +2028,7 @@
       <c r="E35" s="14"/>
       <c r="G35" s="58"/>
       <c r="I35" s="42" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J35" s="42">
         <v>10</v>
@@ -2018,11 +2044,11 @@
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G36" s="58"/>
       <c r="I36" s="45" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J36" s="45">
         <v>10</v>
@@ -2033,11 +2059,11 @@
       <c r="B37" s="35"/>
       <c r="C37" s="35"/>
       <c r="D37" s="48" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E37" s="49">
         <f ca="1">TODAY()</f>
-        <v>41872</v>
+        <v>41884</v>
       </c>
       <c r="G37" s="49"/>
       <c r="J37" s="8">

</xml_diff>

<commit_message>
demo day assignments detailed
</commit_message>
<xml_diff>
--- a/CIS440FALL2014schedule.xlsx
+++ b/CIS440FALL2014schedule.xlsx
@@ -1282,7 +1282,7 @@
   <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,7 +1557,7 @@
         <v>84</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>60</v>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="E37" s="49">
         <f ca="1">TODAY()</f>
-        <v>41894</v>
+        <v>41901</v>
       </c>
       <c r="G37" s="49"/>
       <c r="J37" s="8">

</xml_diff>